<commit_message>
add images and change manual design
</commit_message>
<xml_diff>
--- a/report/evaluation/3-Questionnaire/evaluationResults.xlsx
+++ b/report/evaluation/3-Questionnaire/evaluationResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodos\Documents\GitHub\mis1920\report\evaluation\3-Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6462E64-26EE-4D3E-BF5C-6A0D3FDFD786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B44D68-14CC-4627-ABF8-817CEC18DE47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B2B15ABE-85BF-438D-B0E8-6787108BF709}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Utente</t>
   </si>
@@ -174,6 +174,27 @@
   </si>
   <si>
     <t>Punti e palline più grandi/visibili</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Audio interface</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Non M</t>
   </si>
 </sst>
 </file>
@@ -217,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -453,11 +474,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -539,6 +580,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -856,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284B6B8B-95A6-4008-8916-DF50BF456881}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:R11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1515,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14" s="36"/>
+      <c r="P14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
@@ -1468,6 +1536,14 @@
       <c r="C15" s="4">
         <v>22</v>
       </c>
+      <c r="N15" s="5"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="16">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="34">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1477,8 +1553,16 @@
       <c r="C16" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N16" s="5"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
@@ -1486,8 +1570,16 @@
       <c r="C17" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N17" s="5"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="16">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
@@ -1495,8 +1587,16 @@
       <c r="C18" s="7">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N18" s="5"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1506,15 +1606,35 @@
       <c r="C19" s="7">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N19" s="5"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N20" s="5"/>
+      <c r="O20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P20" s="3">
+        <f>AVERAGE(P15:P19)</f>
+        <v>3</v>
+      </c>
+      <c r="Q20" s="4">
+        <f>AVERAGE(Q15:Q19)</f>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
@@ -1524,8 +1644,20 @@
       <c r="C21" s="7">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N21" s="8"/>
+      <c r="O21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P21" s="9">
+        <f>_xlfn.STDEV.P(P15:P19)</f>
+        <v>1.7888543819998317</v>
+      </c>
+      <c r="Q21" s="10">
+        <f>_xlfn.STDEV.P(Q15:Q19)</f>
+        <v>0.39999999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1536,21 +1668,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6" t="s">
         <v>39</v>
@@ -1559,8 +1697,14 @@
         <f>AVERAGE(C15:C24)</f>
         <v>24.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P25" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="9" t="s">
         <v>40</v>
@@ -1570,37 +1714,86 @@
         <v>4.7169905660283016</v>
       </c>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="P26" s="30">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="P27" s="30">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="Q28" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="Q29" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="Q30" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="Q31" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="O32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P32" s="3">
+        <f>AVERAGE(P25:P27)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="Q32" s="4">
+        <f>AVERAGE(Q25:Q31)</f>
+        <v>3.1428571428571428</v>
+      </c>
+    </row>
+    <row r="33" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="O33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P33" s="9">
+        <f>_xlfn.STDEV.P(P25:P27)</f>
+        <v>0.94280904158206336</v>
+      </c>
+      <c r="Q33" s="10">
+        <f>_xlfn.STDEV.P(Q25:Q31)</f>
+        <v>1.7261494247992246</v>
+      </c>
+    </row>
+    <row r="34" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N14:O14"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>